<commit_message>
Password Policy based on OU
</commit_message>
<xml_diff>
--- a/src/test/resources/input/Login.xlsx
+++ b/src/test/resources/input/Login.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72">
   <si>
     <t>Valid_LoginDetails</t>
   </si>
@@ -228,6 +228,15 @@
   </si>
   <si>
     <t>@#$#</t>
+  </si>
+  <si>
+    <t>VerfiyOUpasswordpolicy</t>
+  </si>
+  <si>
+    <t>UserEmail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test031@demo.cloudnowtech.com	</t>
   </si>
 </sst>
 </file>
@@ -235,13 +244,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="16">
     <font>
       <sz val="11"/>
       <color indexed="50"/>
@@ -255,15 +264,17 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color indexed="52"/>
+      <u/>
+      <sz val="11"/>
+      <color indexed="31"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color indexed="11"/>
+      <b/>
+      <sz val="24"/>
+      <color indexed="50"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -277,31 +288,16 @@
       <charset val="1"/>
     </font>
     <font>
-      <i/>
       <sz val="10"/>
-      <color indexed="15"/>
+      <color indexed="52"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
-      <b/>
-      <sz val="24"/>
-      <color indexed="50"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="18"/>
-      <color indexed="50"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
+      <i/>
       <sz val="10"/>
-      <color indexed="23"/>
+      <color indexed="15"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -321,9 +317,15 @@
       <charset val="1"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color indexed="31"/>
+      <sz val="10"/>
+      <color indexed="23"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color indexed="50"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -336,10 +338,24 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color indexed="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <b/>
       <sz val="10"/>
       <color indexed="23"/>
       <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color indexed="12"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -372,8 +388,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="39"/>
-        <bgColor indexed="23"/>
+        <fgColor indexed="23"/>
+        <bgColor indexed="39"/>
       </patternFill>
     </fill>
     <fill>
@@ -384,20 +400,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="23"/>
-        <bgColor indexed="39"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor indexed="15"/>
         <bgColor indexed="47"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="50"/>
-        <bgColor indexed="50"/>
+        <fgColor indexed="39"/>
+        <bgColor indexed="23"/>
       </patternFill>
     </fill>
     <fill>
@@ -410,6 +420,12 @@
       <patternFill patternType="solid">
         <fgColor indexed="52"/>
         <bgColor indexed="8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="50"/>
+        <bgColor indexed="50"/>
       </patternFill>
     </fill>
   </fills>
@@ -467,7 +483,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="25">
+  <cellStyleXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="top"/>
     </xf>
@@ -489,7 +505,7 @@
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyBorder="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -498,53 +514,59 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyBorder="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyBorder="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="3" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyBorder="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyBorder="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyBorder="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="3" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyBorder="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyBorder="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyBorder="0" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyBorder="0" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyBorder="0" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyBorder="0" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyBorder="0" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyBorder="0" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyBorder="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyBorder="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyBorder="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="top"/>
     </xf>
@@ -563,7 +585,10 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="16" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="25" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="15" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -572,7 +597,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="16" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="15" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -584,7 +609,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -597,7 +622,7 @@
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
-  <cellStyles count="25">
+  <cellStyles count="27">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Text" xfId="2"/>
@@ -610,11 +635,11 @@
     <cellStyle name="Currency[0]" xfId="9" builtinId="7"/>
     <cellStyle name="Heading" xfId="10"/>
     <cellStyle name="Heading 1" xfId="11"/>
-    <cellStyle name="Heading 2" xfId="12"/>
-    <cellStyle name="Note" xfId="13"/>
+    <cellStyle name="Note" xfId="12"/>
+    <cellStyle name="Heading 2" xfId="13"/>
     <cellStyle name="Footnote" xfId="14"/>
-    <cellStyle name="Status" xfId="15"/>
-    <cellStyle name="*unknown*" xfId="16"/>
+    <cellStyle name="*unknown*" xfId="15"/>
+    <cellStyle name="Status" xfId="16"/>
     <cellStyle name="Good" xfId="17"/>
     <cellStyle name="Neutral" xfId="18"/>
     <cellStyle name="Bad" xfId="19"/>
@@ -623,6 +648,8 @@
     <cellStyle name="Accent" xfId="22"/>
     <cellStyle name="Accent 1" xfId="23"/>
     <cellStyle name="Accent 2" xfId="24"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -1057,7 +1084,7 @@
     </row>
     <row r="7" spans="2:5">
       <c r="B7" s="2"/>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="7" t="s">
         <v>3</v>
       </c>
       <c r="D7" s="2" t="s">
@@ -1087,7 +1114,7 @@
     </row>
     <row r="13" spans="2:5">
       <c r="B13" s="2"/>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="7" t="s">
         <v>6</v>
       </c>
       <c r="D13" s="2" t="s">
@@ -1117,7 +1144,7 @@
     </row>
     <row r="19" spans="2:5">
       <c r="B19" s="2"/>
-      <c r="C19" s="6" t="s">
+      <c r="C19" s="7" t="s">
         <v>3</v>
       </c>
       <c r="D19" s="2" t="s">
@@ -1135,9 +1162,9 @@
     </row>
   </sheetData>
   <hyperlinks>
+    <hyperlink ref="C19" r:id="rId1" display="qa@demo.cloudnowtech.com"/>
+    <hyperlink ref="C13" r:id="rId2" display="invalidEmail@demo.cloudnowtech.com"/>
     <hyperlink ref="C7" r:id="rId1" display="qa@demo.cloudnowtech.com"/>
-    <hyperlink ref="C13" r:id="rId2" display="invalidEmail@demo.cloudnowtech.com"/>
-    <hyperlink ref="C19" r:id="rId1" display="qa@demo.cloudnowtech.com"/>
   </hyperlinks>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.510416666666667" footer="0.510416666666667"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
@@ -1167,279 +1194,279 @@
   </cols>
   <sheetData>
     <row r="9" spans="2:10">
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="E9" s="7" t="s">
+      <c r="C9" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="F9" s="7" t="s">
+      <c r="F9" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G9" s="7" t="s">
+      <c r="G9" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="H9" s="8"/>
-      <c r="I9" s="15"/>
-      <c r="J9" s="16"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="16"/>
+      <c r="J9" s="17"/>
     </row>
     <row r="10" spans="2:10">
-      <c r="B10" s="8"/>
-      <c r="C10" s="9" t="s">
+      <c r="B10" s="9"/>
+      <c r="C10" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="D10" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="E10" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="F10" s="10" t="s">
+      <c r="D10" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="F10" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="G10" s="10" t="s">
+      <c r="G10" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="H10" s="8"/>
-      <c r="I10" s="16"/>
-      <c r="J10" s="16"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="17"/>
+      <c r="J10" s="17"/>
     </row>
     <row r="11" spans="2:10">
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="7" t="s">
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="I11" s="16"/>
-      <c r="J11" s="16"/>
+      <c r="I11" s="17"/>
+      <c r="J11" s="17"/>
     </row>
     <row r="12" spans="9:10">
-      <c r="I12" s="16"/>
-      <c r="J12" s="16"/>
+      <c r="I12" s="17"/>
+      <c r="J12" s="17"/>
     </row>
     <row r="13" spans="2:10">
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="E13" s="7" t="s">
+      <c r="C13" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E13" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="F13" s="7" t="s">
+      <c r="F13" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G13" s="7" t="s">
+      <c r="G13" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="H13" s="8"/>
-      <c r="I13" s="15"/>
-      <c r="J13" s="15"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="16"/>
+      <c r="J13" s="16"/>
     </row>
     <row r="14" spans="2:8">
-      <c r="B14" s="8"/>
-      <c r="C14" s="9" t="s">
+      <c r="B14" s="9"/>
+      <c r="C14" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="D14" s="10" t="s">
+      <c r="D14" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="E14" s="10" t="s">
+      <c r="E14" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="F14" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="G14" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="H14" s="8"/>
+      <c r="F14" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="G14" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="H14" s="9"/>
     </row>
     <row r="15" spans="2:8">
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="7" t="s">
+      <c r="B15" s="9"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="8" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="18" spans="2:8">
-      <c r="B18" s="7" t="s">
+      <c r="B18" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="E18" s="7" t="s">
+      <c r="C18" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E18" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="F18" s="7" t="s">
+      <c r="F18" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G18" s="7" t="s">
+      <c r="G18" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="H18" s="8"/>
+      <c r="H18" s="9"/>
     </row>
     <row r="19" spans="2:8">
-      <c r="B19" s="8"/>
-      <c r="C19" s="9" t="s">
+      <c r="B19" s="9"/>
+      <c r="C19" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="D19" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="E19" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="F19" s="10" t="s">
+      <c r="D19" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="E19" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="F19" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="G19" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="H19" s="8"/>
+      <c r="G19" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="H19" s="9"/>
     </row>
     <row r="20" spans="2:8">
-      <c r="B20" s="8"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="8"/>
-      <c r="G20" s="8"/>
-      <c r="H20" s="7" t="s">
+      <c r="B20" s="9"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="8" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="22" spans="2:8">
-      <c r="B22" s="7" t="s">
+      <c r="B22" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C22" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D22" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="E22" s="7" t="s">
+      <c r="C22" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E22" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="F22" s="7" t="s">
+      <c r="F22" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G22" s="7" t="s">
+      <c r="G22" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="H22" s="8"/>
+      <c r="H22" s="9"/>
     </row>
     <row r="23" spans="2:8">
-      <c r="B23" s="8"/>
-      <c r="C23" s="9" t="s">
+      <c r="B23" s="9"/>
+      <c r="C23" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="D23" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="E23" s="10" t="s">
+      <c r="D23" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="E23" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="F23" s="10" t="s">
+      <c r="F23" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="G23" s="10" t="s">
+      <c r="G23" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="H23" s="8"/>
+      <c r="H23" s="9"/>
     </row>
     <row r="24" spans="2:8">
-      <c r="B24" s="8"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="8"/>
-      <c r="E24" s="8"/>
-      <c r="F24" s="8"/>
-      <c r="G24" s="8"/>
-      <c r="H24" s="7" t="s">
+      <c r="B24" s="9"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="9"/>
+      <c r="G24" s="9"/>
+      <c r="H24" s="8" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="26" ht="30" spans="2:8">
-      <c r="B26" s="14" t="s">
+      <c r="B26" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="C26" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D26" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="E26" s="7" t="s">
+      <c r="C26" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D26" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E26" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="F26" s="7" t="s">
+      <c r="F26" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G26" s="7" t="s">
+      <c r="G26" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="H26" s="8"/>
+      <c r="H26" s="9"/>
     </row>
     <row r="27" spans="2:8">
-      <c r="B27" s="8"/>
-      <c r="C27" s="9" t="s">
+      <c r="B27" s="9"/>
+      <c r="C27" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="D27" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="E27" s="10" t="s">
+      <c r="D27" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="E27" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="F27" s="10" t="s">
+      <c r="F27" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="G27" s="10" t="s">
+      <c r="G27" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="H27" s="8"/>
+      <c r="H27" s="9"/>
     </row>
     <row r="28" ht="30" spans="2:8">
-      <c r="B28" s="8"/>
-      <c r="C28" s="8"/>
-      <c r="D28" s="8"/>
-      <c r="E28" s="8"/>
-      <c r="F28" s="8"/>
-      <c r="G28" s="8"/>
-      <c r="H28" s="14" t="s">
+      <c r="B28" s="9"/>
+      <c r="C28" s="9"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="9"/>
+      <c r="G28" s="9"/>
+      <c r="H28" s="15" t="s">
         <v>18</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
+    <hyperlink ref="C27" r:id="rId1" display="qa@demo.cloudnowtech.com"/>
+    <hyperlink ref="C23" r:id="rId1" display="qa@demo.cloudnowtech.com"/>
+    <hyperlink ref="C19" r:id="rId1" display="qa@demo.cloudnowtech.com"/>
+    <hyperlink ref="C14" r:id="rId1" display="qa@demo.cloudnowtech.com"/>
     <hyperlink ref="C10" r:id="rId1" display="qa@demo.cloudnowtech.com"/>
-    <hyperlink ref="C14" r:id="rId1" display="qa@demo.cloudnowtech.com"/>
-    <hyperlink ref="C19" r:id="rId1" display="qa@demo.cloudnowtech.com"/>
-    <hyperlink ref="C23" r:id="rId1" display="qa@demo.cloudnowtech.com"/>
-    <hyperlink ref="C27" r:id="rId1" display="qa@demo.cloudnowtech.com"/>
   </hyperlinks>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.510416666666667" footer="0.510416666666667"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
@@ -1484,13 +1511,13 @@
     </row>
     <row r="8" spans="3:7">
       <c r="C8" s="2"/>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="7" t="s">
         <v>3</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F8" s="13" t="s">
+      <c r="F8" s="14" t="s">
         <v>21</v>
       </c>
       <c r="G8" s="2"/>
@@ -1506,8 +1533,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D8" r:id="rId1" display="qa@demo.cloudnowtech.com"/>
-    <hyperlink ref="F8" r:id="rId2" display="qacsv@demo.cloudnowtech.com"/>
+    <hyperlink ref="F8" r:id="rId1" display="qacsv@demo.cloudnowtech.com"/>
+    <hyperlink ref="D8" r:id="rId2" display="qa@demo.cloudnowtech.com"/>
   </hyperlinks>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.510416666666667" footer="0.510416666666667"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
@@ -1556,7 +1583,7 @@
     </row>
     <row r="6" spans="2:7">
       <c r="B6" s="2"/>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="7" t="s">
         <v>3</v>
       </c>
       <c r="D6" s="2" t="s">
@@ -1600,7 +1627,7 @@
     </row>
     <row r="10" spans="2:7">
       <c r="B10" s="2"/>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="7" t="s">
         <v>3</v>
       </c>
       <c r="D10" s="2" t="s">
@@ -1643,7 +1670,7 @@
     </row>
     <row r="16" spans="2:7">
       <c r="B16" s="2"/>
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="7" t="s">
         <v>3</v>
       </c>
       <c r="D16" s="2" t="s">
@@ -1686,7 +1713,7 @@
     </row>
     <row r="22" spans="2:7">
       <c r="B22" s="2"/>
-      <c r="C22" s="6" t="s">
+      <c r="C22" s="7" t="s">
         <v>3</v>
       </c>
       <c r="D22" s="2" t="s">
@@ -1712,12 +1739,12 @@
     </row>
   </sheetData>
   <hyperlinks>
+    <hyperlink ref="C22" r:id="rId1" display="qa@demo.cloudnowtech.com"/>
+    <hyperlink ref="C16" r:id="rId1" display="qa@demo.cloudnowtech.com"/>
+    <hyperlink ref="E10" r:id="rId2" display="www.yahoo.com"/>
+    <hyperlink ref="C10" r:id="rId1" display="qa@demo.cloudnowtech.com"/>
+    <hyperlink ref="E6" r:id="rId3" display="www.google.com"/>
     <hyperlink ref="C6" r:id="rId1" display="qa@demo.cloudnowtech.com"/>
-    <hyperlink ref="E6" r:id="rId2" display="www.google.com"/>
-    <hyperlink ref="C10" r:id="rId1" display="qa@demo.cloudnowtech.com"/>
-    <hyperlink ref="E10" r:id="rId3" display="www.yahoo.com"/>
-    <hyperlink ref="C16" r:id="rId1" display="qa@demo.cloudnowtech.com"/>
-    <hyperlink ref="C22" r:id="rId1" display="qa@demo.cloudnowtech.com"/>
   </hyperlinks>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
@@ -1752,119 +1779,119 @@
   </cols>
   <sheetData>
     <row r="7" spans="2:8">
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C7" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="E7" s="7" t="s">
+      <c r="C7" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="F7" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="G7" s="7" t="s">
+      <c r="G7" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="H7" s="8"/>
+      <c r="H7" s="9"/>
     </row>
     <row r="8" spans="2:8">
-      <c r="B8" s="11"/>
-      <c r="C8" s="10" t="s">
+      <c r="B8" s="12"/>
+      <c r="C8" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="E8" s="10" t="s">
+      <c r="D8" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="E8" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="F8" s="11" t="s">
+      <c r="F8" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="G8" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="H8" s="8"/>
+      <c r="G8" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="H8" s="9"/>
     </row>
     <row r="9" spans="2:8">
-      <c r="B9" s="12"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="7" t="s">
+      <c r="B9" s="13"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="8" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="12" spans="2:9">
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C12" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="E12" s="7" t="s">
+      <c r="C12" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E12" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="F12" s="7" t="s">
+      <c r="F12" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="G12" s="7" t="s">
+      <c r="G12" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="H12" s="7" t="s">
+      <c r="H12" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="I12" s="8"/>
+      <c r="I12" s="9"/>
     </row>
     <row r="13" spans="2:9">
-      <c r="B13" s="8"/>
-      <c r="C13" s="10" t="s">
+      <c r="B13" s="9"/>
+      <c r="C13" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="D13" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="E13" s="10" t="s">
+      <c r="D13" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="E13" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="F13" s="10" t="s">
+      <c r="F13" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="G13" s="10" t="s">
+      <c r="G13" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="H13" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="I13" s="8"/>
+      <c r="H13" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="I13" s="9"/>
     </row>
     <row r="14" spans="2:9">
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="8"/>
-      <c r="I14" s="7" t="s">
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="8" t="s">
         <v>38</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C8" r:id="rId1" display="qa@demo.cloudnowtech.com"/>
-    <hyperlink ref="C13" r:id="rId1" display="qa@demo.cloudnowtech.com"/>
-    <hyperlink ref="E13" r:id="rId2" display="mathi.t@demo.cloudnowtech.com"/>
+    <hyperlink ref="E13" r:id="rId1" display="mathi.t@demo.cloudnowtech.com"/>
+    <hyperlink ref="C13" r:id="rId2" display="qa@demo.cloudnowtech.com"/>
+    <hyperlink ref="C8" r:id="rId2" display="qa@demo.cloudnowtech.com"/>
   </hyperlinks>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
@@ -1971,7 +1998,7 @@
     </row>
     <row r="12" spans="2:8">
       <c r="B12" s="2"/>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="7" t="s">
         <v>3</v>
       </c>
       <c r="D12" s="2" t="s">
@@ -2000,60 +2027,60 @@
       </c>
     </row>
     <row r="16" spans="2:9">
-      <c r="B16" s="7" t="s">
+      <c r="B16" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="E16" s="7" t="s">
+      <c r="C16" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E16" s="8" t="s">
         <v>10</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="G16" s="7" t="s">
+      <c r="G16" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="H16" s="7" t="s">
+      <c r="H16" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="I16" s="8"/>
+      <c r="I16" s="9"/>
     </row>
     <row r="17" spans="2:9">
-      <c r="B17" s="8"/>
-      <c r="C17" s="9" t="s">
+      <c r="B17" s="9"/>
+      <c r="C17" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="D17" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="E17" s="10" t="s">
+      <c r="D17" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="E17" s="11" t="s">
         <v>4</v>
       </c>
       <c r="F17" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="G17" s="10" t="s">
+      <c r="G17" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="H17" s="10" t="s">
+      <c r="H17" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="I17" s="8"/>
+      <c r="I17" s="9"/>
     </row>
     <row r="18" spans="2:9">
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="8"/>
-      <c r="I18" s="7" t="s">
+      <c r="B18" s="9"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="8" t="s">
         <v>9</v>
       </c>
     </row>
@@ -2161,12 +2188,12 @@
     </row>
   </sheetData>
   <hyperlinks>
+    <hyperlink ref="C25" r:id="rId1" display="qa@demo.cloudnowtech.com"/>
+    <hyperlink ref="C21" r:id="rId1" display="qa@demo.cloudnowtech.com"/>
+    <hyperlink ref="C17" r:id="rId1" display="qa@demo.cloudnowtech.com"/>
+    <hyperlink ref="C12" r:id="rId1" display="qa@demo.cloudnowtech.com"/>
+    <hyperlink ref="G7" r:id="rId2" display="test50@demo.cloudnowtech.com"/>
     <hyperlink ref="C7" r:id="rId1" display="qa@demo.cloudnowtech.com"/>
-    <hyperlink ref="G7" r:id="rId2" display="test50@demo.cloudnowtech.com"/>
-    <hyperlink ref="C12" r:id="rId1" display="qa@demo.cloudnowtech.com"/>
-    <hyperlink ref="C17" r:id="rId1" display="qa@demo.cloudnowtech.com"/>
-    <hyperlink ref="C21" r:id="rId1" display="qa@demo.cloudnowtech.com"/>
-    <hyperlink ref="C25" r:id="rId1" display="qa@demo.cloudnowtech.com"/>
   </hyperlinks>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
@@ -2180,13 +2207,13 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="B7:G31"/>
+  <dimension ref="B7:H35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="H37" sqref="H37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="7"/>
   <cols>
     <col min="2" max="2" width="34.8571428571429" customWidth="1"/>
     <col min="3" max="3" width="30.4285714285714" customWidth="1"/>
@@ -2194,6 +2221,7 @@
     <col min="5" max="5" width="17.4285714285714" customWidth="1"/>
     <col min="6" max="6" width="16.8571428571429" customWidth="1"/>
     <col min="7" max="7" width="34.8571428571429" customWidth="1"/>
+    <col min="8" max="8" width="31.7142857142857" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="7" spans="2:7">
@@ -2460,14 +2488,67 @@
         <v>67</v>
       </c>
     </row>
+    <row r="33" spans="2:8">
+      <c r="B33" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="H33" s="2"/>
+    </row>
+    <row r="34" spans="2:8">
+      <c r="B34" s="2"/>
+      <c r="C34" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G34" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="H34" s="2"/>
+    </row>
+    <row r="35" spans="2:8">
+      <c r="B35" s="5"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="5"/>
+      <c r="F35" s="5"/>
+      <c r="G35" s="5"/>
+      <c r="H35" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C8" r:id="rId1" display="qa@demo.cloudnowtech.com"/>
-    <hyperlink ref="C26" r:id="rId1" display="qa@demo.cloudnowtech.com"/>
-    <hyperlink ref="C12" r:id="rId1" display="qa@demo.cloudnowtech.com"/>
-    <hyperlink ref="C30" r:id="rId1" display="qa@demo.cloudnowtech.com"/>
-    <hyperlink ref="C16" r:id="rId1" display="qa@demo.cloudnowtech.com"/>
-    <hyperlink ref="C20" r:id="rId1" display="qa@demo.cloudnowtech.com"/>
+    <hyperlink ref="G34" r:id="rId1" display="test031@demo.cloudnowtech.com " tooltip="mailto:test031@demo.cloudnowtech.com "/>
+    <hyperlink ref="C34" r:id="rId2" display="qa@demo.cloudnowtech.com"/>
+    <hyperlink ref="C20" r:id="rId2" display="qa@demo.cloudnowtech.com"/>
+    <hyperlink ref="C16" r:id="rId2" display="qa@demo.cloudnowtech.com"/>
+    <hyperlink ref="C30" r:id="rId2" display="qa@demo.cloudnowtech.com"/>
+    <hyperlink ref="C12" r:id="rId2" display="qa@demo.cloudnowtech.com"/>
+    <hyperlink ref="C26" r:id="rId2" display="qa@demo.cloudnowtech.com"/>
+    <hyperlink ref="C8" r:id="rId2" display="qa@demo.cloudnowtech.com"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>

<commit_message>
With Extended Report Setup In Login
</commit_message>
<xml_diff>
--- a/src/test/resources/input/Login.xlsx
+++ b/src/test/resources/input/Login.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72">
   <si>
     <t>Valid_LoginDetails</t>
   </si>
@@ -228,6 +228,15 @@
   </si>
   <si>
     <t>@#$#</t>
+  </si>
+  <si>
+    <t>VerfiyOUpasswordpolicy</t>
+  </si>
+  <si>
+    <t>UserEmail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test031@demo.cloudnowtech.com	</t>
   </si>
 </sst>
 </file>
@@ -235,13 +244,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="16">
     <font>
       <sz val="11"/>
       <color indexed="50"/>
@@ -255,15 +264,17 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color indexed="52"/>
+      <u/>
+      <sz val="11"/>
+      <color indexed="31"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color indexed="11"/>
+      <b/>
+      <sz val="24"/>
+      <color indexed="50"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -277,31 +288,16 @@
       <charset val="1"/>
     </font>
     <font>
-      <i/>
       <sz val="10"/>
-      <color indexed="15"/>
+      <color indexed="52"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
-      <b/>
-      <sz val="24"/>
-      <color indexed="50"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="18"/>
-      <color indexed="50"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
+      <i/>
       <sz val="10"/>
-      <color indexed="23"/>
+      <color indexed="15"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -321,9 +317,15 @@
       <charset val="1"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color indexed="31"/>
+      <sz val="10"/>
+      <color indexed="23"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color indexed="50"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -336,10 +338,24 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color indexed="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <b/>
       <sz val="10"/>
       <color indexed="23"/>
       <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color indexed="12"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -372,8 +388,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="39"/>
-        <bgColor indexed="23"/>
+        <fgColor indexed="23"/>
+        <bgColor indexed="39"/>
       </patternFill>
     </fill>
     <fill>
@@ -384,20 +400,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="23"/>
-        <bgColor indexed="39"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor indexed="15"/>
         <bgColor indexed="47"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="50"/>
-        <bgColor indexed="50"/>
+        <fgColor indexed="39"/>
+        <bgColor indexed="23"/>
       </patternFill>
     </fill>
     <fill>
@@ -410,6 +420,12 @@
       <patternFill patternType="solid">
         <fgColor indexed="52"/>
         <bgColor indexed="8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="50"/>
+        <bgColor indexed="50"/>
       </patternFill>
     </fill>
   </fills>
@@ -467,7 +483,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="25">
+  <cellStyleXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="top"/>
     </xf>
@@ -489,7 +505,7 @@
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyBorder="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -498,53 +514,59 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyBorder="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyBorder="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="3" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyBorder="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyBorder="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyBorder="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="3" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyBorder="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyBorder="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyBorder="0" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyBorder="0" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyBorder="0" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyBorder="0" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyBorder="0" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyBorder="0" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyBorder="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyBorder="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyBorder="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="top"/>
     </xf>
@@ -563,7 +585,10 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="16" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="25" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="15" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -572,7 +597,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="16" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="15" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -584,7 +609,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -597,7 +622,7 @@
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
-  <cellStyles count="25">
+  <cellStyles count="27">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Text" xfId="2"/>
@@ -610,11 +635,11 @@
     <cellStyle name="Currency[0]" xfId="9" builtinId="7"/>
     <cellStyle name="Heading" xfId="10"/>
     <cellStyle name="Heading 1" xfId="11"/>
-    <cellStyle name="Heading 2" xfId="12"/>
-    <cellStyle name="Note" xfId="13"/>
+    <cellStyle name="Note" xfId="12"/>
+    <cellStyle name="Heading 2" xfId="13"/>
     <cellStyle name="Footnote" xfId="14"/>
-    <cellStyle name="Status" xfId="15"/>
-    <cellStyle name="*unknown*" xfId="16"/>
+    <cellStyle name="*unknown*" xfId="15"/>
+    <cellStyle name="Status" xfId="16"/>
     <cellStyle name="Good" xfId="17"/>
     <cellStyle name="Neutral" xfId="18"/>
     <cellStyle name="Bad" xfId="19"/>
@@ -623,6 +648,8 @@
     <cellStyle name="Accent" xfId="22"/>
     <cellStyle name="Accent 1" xfId="23"/>
     <cellStyle name="Accent 2" xfId="24"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -1057,7 +1084,7 @@
     </row>
     <row r="7" spans="2:5">
       <c r="B7" s="2"/>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="7" t="s">
         <v>3</v>
       </c>
       <c r="D7" s="2" t="s">
@@ -1087,7 +1114,7 @@
     </row>
     <row r="13" spans="2:5">
       <c r="B13" s="2"/>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="7" t="s">
         <v>6</v>
       </c>
       <c r="D13" s="2" t="s">
@@ -1117,7 +1144,7 @@
     </row>
     <row r="19" spans="2:5">
       <c r="B19" s="2"/>
-      <c r="C19" s="6" t="s">
+      <c r="C19" s="7" t="s">
         <v>3</v>
       </c>
       <c r="D19" s="2" t="s">
@@ -1135,9 +1162,9 @@
     </row>
   </sheetData>
   <hyperlinks>
+    <hyperlink ref="C19" r:id="rId1" display="qa@demo.cloudnowtech.com"/>
+    <hyperlink ref="C13" r:id="rId2" display="invalidEmail@demo.cloudnowtech.com"/>
     <hyperlink ref="C7" r:id="rId1" display="qa@demo.cloudnowtech.com"/>
-    <hyperlink ref="C13" r:id="rId2" display="invalidEmail@demo.cloudnowtech.com"/>
-    <hyperlink ref="C19" r:id="rId1" display="qa@demo.cloudnowtech.com"/>
   </hyperlinks>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.510416666666667" footer="0.510416666666667"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
@@ -1167,279 +1194,279 @@
   </cols>
   <sheetData>
     <row r="9" spans="2:10">
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="E9" s="7" t="s">
+      <c r="C9" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="F9" s="7" t="s">
+      <c r="F9" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G9" s="7" t="s">
+      <c r="G9" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="H9" s="8"/>
-      <c r="I9" s="15"/>
-      <c r="J9" s="16"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="16"/>
+      <c r="J9" s="17"/>
     </row>
     <row r="10" spans="2:10">
-      <c r="B10" s="8"/>
-      <c r="C10" s="9" t="s">
+      <c r="B10" s="9"/>
+      <c r="C10" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="D10" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="E10" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="F10" s="10" t="s">
+      <c r="D10" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="F10" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="G10" s="10" t="s">
+      <c r="G10" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="H10" s="8"/>
-      <c r="I10" s="16"/>
-      <c r="J10" s="16"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="17"/>
+      <c r="J10" s="17"/>
     </row>
     <row r="11" spans="2:10">
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="7" t="s">
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="I11" s="16"/>
-      <c r="J11" s="16"/>
+      <c r="I11" s="17"/>
+      <c r="J11" s="17"/>
     </row>
     <row r="12" spans="9:10">
-      <c r="I12" s="16"/>
-      <c r="J12" s="16"/>
+      <c r="I12" s="17"/>
+      <c r="J12" s="17"/>
     </row>
     <row r="13" spans="2:10">
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="E13" s="7" t="s">
+      <c r="C13" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E13" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="F13" s="7" t="s">
+      <c r="F13" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G13" s="7" t="s">
+      <c r="G13" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="H13" s="8"/>
-      <c r="I13" s="15"/>
-      <c r="J13" s="15"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="16"/>
+      <c r="J13" s="16"/>
     </row>
     <row r="14" spans="2:8">
-      <c r="B14" s="8"/>
-      <c r="C14" s="9" t="s">
+      <c r="B14" s="9"/>
+      <c r="C14" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="D14" s="10" t="s">
+      <c r="D14" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="E14" s="10" t="s">
+      <c r="E14" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="F14" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="G14" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="H14" s="8"/>
+      <c r="F14" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="G14" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="H14" s="9"/>
     </row>
     <row r="15" spans="2:8">
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="7" t="s">
+      <c r="B15" s="9"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="8" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="18" spans="2:8">
-      <c r="B18" s="7" t="s">
+      <c r="B18" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="E18" s="7" t="s">
+      <c r="C18" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E18" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="F18" s="7" t="s">
+      <c r="F18" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G18" s="7" t="s">
+      <c r="G18" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="H18" s="8"/>
+      <c r="H18" s="9"/>
     </row>
     <row r="19" spans="2:8">
-      <c r="B19" s="8"/>
-      <c r="C19" s="9" t="s">
+      <c r="B19" s="9"/>
+      <c r="C19" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="D19" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="E19" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="F19" s="10" t="s">
+      <c r="D19" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="E19" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="F19" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="G19" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="H19" s="8"/>
+      <c r="G19" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="H19" s="9"/>
     </row>
     <row r="20" spans="2:8">
-      <c r="B20" s="8"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="8"/>
-      <c r="G20" s="8"/>
-      <c r="H20" s="7" t="s">
+      <c r="B20" s="9"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="8" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="22" spans="2:8">
-      <c r="B22" s="7" t="s">
+      <c r="B22" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C22" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D22" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="E22" s="7" t="s">
+      <c r="C22" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E22" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="F22" s="7" t="s">
+      <c r="F22" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G22" s="7" t="s">
+      <c r="G22" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="H22" s="8"/>
+      <c r="H22" s="9"/>
     </row>
     <row r="23" spans="2:8">
-      <c r="B23" s="8"/>
-      <c r="C23" s="9" t="s">
+      <c r="B23" s="9"/>
+      <c r="C23" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="D23" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="E23" s="10" t="s">
+      <c r="D23" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="E23" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="F23" s="10" t="s">
+      <c r="F23" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="G23" s="10" t="s">
+      <c r="G23" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="H23" s="8"/>
+      <c r="H23" s="9"/>
     </row>
     <row r="24" spans="2:8">
-      <c r="B24" s="8"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="8"/>
-      <c r="E24" s="8"/>
-      <c r="F24" s="8"/>
-      <c r="G24" s="8"/>
-      <c r="H24" s="7" t="s">
+      <c r="B24" s="9"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="9"/>
+      <c r="G24" s="9"/>
+      <c r="H24" s="8" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="26" ht="30" spans="2:8">
-      <c r="B26" s="14" t="s">
+      <c r="B26" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="C26" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D26" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="E26" s="7" t="s">
+      <c r="C26" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D26" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E26" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="F26" s="7" t="s">
+      <c r="F26" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G26" s="7" t="s">
+      <c r="G26" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="H26" s="8"/>
+      <c r="H26" s="9"/>
     </row>
     <row r="27" spans="2:8">
-      <c r="B27" s="8"/>
-      <c r="C27" s="9" t="s">
+      <c r="B27" s="9"/>
+      <c r="C27" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="D27" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="E27" s="10" t="s">
+      <c r="D27" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="E27" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="F27" s="10" t="s">
+      <c r="F27" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="G27" s="10" t="s">
+      <c r="G27" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="H27" s="8"/>
+      <c r="H27" s="9"/>
     </row>
     <row r="28" ht="30" spans="2:8">
-      <c r="B28" s="8"/>
-      <c r="C28" s="8"/>
-      <c r="D28" s="8"/>
-      <c r="E28" s="8"/>
-      <c r="F28" s="8"/>
-      <c r="G28" s="8"/>
-      <c r="H28" s="14" t="s">
+      <c r="B28" s="9"/>
+      <c r="C28" s="9"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="9"/>
+      <c r="G28" s="9"/>
+      <c r="H28" s="15" t="s">
         <v>18</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
+    <hyperlink ref="C27" r:id="rId1" display="qa@demo.cloudnowtech.com"/>
+    <hyperlink ref="C23" r:id="rId1" display="qa@demo.cloudnowtech.com"/>
+    <hyperlink ref="C19" r:id="rId1" display="qa@demo.cloudnowtech.com"/>
+    <hyperlink ref="C14" r:id="rId1" display="qa@demo.cloudnowtech.com"/>
     <hyperlink ref="C10" r:id="rId1" display="qa@demo.cloudnowtech.com"/>
-    <hyperlink ref="C14" r:id="rId1" display="qa@demo.cloudnowtech.com"/>
-    <hyperlink ref="C19" r:id="rId1" display="qa@demo.cloudnowtech.com"/>
-    <hyperlink ref="C23" r:id="rId1" display="qa@demo.cloudnowtech.com"/>
-    <hyperlink ref="C27" r:id="rId1" display="qa@demo.cloudnowtech.com"/>
   </hyperlinks>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.510416666666667" footer="0.510416666666667"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
@@ -1484,13 +1511,13 @@
     </row>
     <row r="8" spans="3:7">
       <c r="C8" s="2"/>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="7" t="s">
         <v>3</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F8" s="13" t="s">
+      <c r="F8" s="14" t="s">
         <v>21</v>
       </c>
       <c r="G8" s="2"/>
@@ -1506,8 +1533,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D8" r:id="rId1" display="qa@demo.cloudnowtech.com"/>
-    <hyperlink ref="F8" r:id="rId2" display="qacsv@demo.cloudnowtech.com"/>
+    <hyperlink ref="F8" r:id="rId1" display="qacsv@demo.cloudnowtech.com"/>
+    <hyperlink ref="D8" r:id="rId2" display="qa@demo.cloudnowtech.com"/>
   </hyperlinks>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.510416666666667" footer="0.510416666666667"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
@@ -1556,7 +1583,7 @@
     </row>
     <row r="6" spans="2:7">
       <c r="B6" s="2"/>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="7" t="s">
         <v>3</v>
       </c>
       <c r="D6" s="2" t="s">
@@ -1600,7 +1627,7 @@
     </row>
     <row r="10" spans="2:7">
       <c r="B10" s="2"/>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="7" t="s">
         <v>3</v>
       </c>
       <c r="D10" s="2" t="s">
@@ -1643,7 +1670,7 @@
     </row>
     <row r="16" spans="2:7">
       <c r="B16" s="2"/>
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="7" t="s">
         <v>3</v>
       </c>
       <c r="D16" s="2" t="s">
@@ -1686,7 +1713,7 @@
     </row>
     <row r="22" spans="2:7">
       <c r="B22" s="2"/>
-      <c r="C22" s="6" t="s">
+      <c r="C22" s="7" t="s">
         <v>3</v>
       </c>
       <c r="D22" s="2" t="s">
@@ -1712,12 +1739,12 @@
     </row>
   </sheetData>
   <hyperlinks>
+    <hyperlink ref="C22" r:id="rId1" display="qa@demo.cloudnowtech.com"/>
+    <hyperlink ref="C16" r:id="rId1" display="qa@demo.cloudnowtech.com"/>
+    <hyperlink ref="E10" r:id="rId2" display="www.yahoo.com"/>
+    <hyperlink ref="C10" r:id="rId1" display="qa@demo.cloudnowtech.com"/>
+    <hyperlink ref="E6" r:id="rId3" display="www.google.com"/>
     <hyperlink ref="C6" r:id="rId1" display="qa@demo.cloudnowtech.com"/>
-    <hyperlink ref="E6" r:id="rId2" display="www.google.com"/>
-    <hyperlink ref="C10" r:id="rId1" display="qa@demo.cloudnowtech.com"/>
-    <hyperlink ref="E10" r:id="rId3" display="www.yahoo.com"/>
-    <hyperlink ref="C16" r:id="rId1" display="qa@demo.cloudnowtech.com"/>
-    <hyperlink ref="C22" r:id="rId1" display="qa@demo.cloudnowtech.com"/>
   </hyperlinks>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
@@ -1752,119 +1779,119 @@
   </cols>
   <sheetData>
     <row r="7" spans="2:8">
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C7" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="E7" s="7" t="s">
+      <c r="C7" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="F7" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="G7" s="7" t="s">
+      <c r="G7" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="H7" s="8"/>
+      <c r="H7" s="9"/>
     </row>
     <row r="8" spans="2:8">
-      <c r="B8" s="11"/>
-      <c r="C8" s="10" t="s">
+      <c r="B8" s="12"/>
+      <c r="C8" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="E8" s="10" t="s">
+      <c r="D8" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="E8" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="F8" s="11" t="s">
+      <c r="F8" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="G8" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="H8" s="8"/>
+      <c r="G8" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="H8" s="9"/>
     </row>
     <row r="9" spans="2:8">
-      <c r="B9" s="12"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="7" t="s">
+      <c r="B9" s="13"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="8" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="12" spans="2:9">
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C12" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="E12" s="7" t="s">
+      <c r="C12" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E12" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="F12" s="7" t="s">
+      <c r="F12" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="G12" s="7" t="s">
+      <c r="G12" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="H12" s="7" t="s">
+      <c r="H12" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="I12" s="8"/>
+      <c r="I12" s="9"/>
     </row>
     <row r="13" spans="2:9">
-      <c r="B13" s="8"/>
-      <c r="C13" s="10" t="s">
+      <c r="B13" s="9"/>
+      <c r="C13" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="D13" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="E13" s="10" t="s">
+      <c r="D13" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="E13" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="F13" s="10" t="s">
+      <c r="F13" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="G13" s="10" t="s">
+      <c r="G13" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="H13" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="I13" s="8"/>
+      <c r="H13" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="I13" s="9"/>
     </row>
     <row r="14" spans="2:9">
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="8"/>
-      <c r="I14" s="7" t="s">
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="8" t="s">
         <v>38</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C8" r:id="rId1" display="qa@demo.cloudnowtech.com"/>
-    <hyperlink ref="C13" r:id="rId1" display="qa@demo.cloudnowtech.com"/>
-    <hyperlink ref="E13" r:id="rId2" display="mathi.t@demo.cloudnowtech.com"/>
+    <hyperlink ref="E13" r:id="rId1" display="mathi.t@demo.cloudnowtech.com"/>
+    <hyperlink ref="C13" r:id="rId2" display="qa@demo.cloudnowtech.com"/>
+    <hyperlink ref="C8" r:id="rId2" display="qa@demo.cloudnowtech.com"/>
   </hyperlinks>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
@@ -1971,7 +1998,7 @@
     </row>
     <row r="12" spans="2:8">
       <c r="B12" s="2"/>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="7" t="s">
         <v>3</v>
       </c>
       <c r="D12" s="2" t="s">
@@ -2000,60 +2027,60 @@
       </c>
     </row>
     <row r="16" spans="2:9">
-      <c r="B16" s="7" t="s">
+      <c r="B16" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="E16" s="7" t="s">
+      <c r="C16" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E16" s="8" t="s">
         <v>10</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="G16" s="7" t="s">
+      <c r="G16" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="H16" s="7" t="s">
+      <c r="H16" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="I16" s="8"/>
+      <c r="I16" s="9"/>
     </row>
     <row r="17" spans="2:9">
-      <c r="B17" s="8"/>
-      <c r="C17" s="9" t="s">
+      <c r="B17" s="9"/>
+      <c r="C17" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="D17" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="E17" s="10" t="s">
+      <c r="D17" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="E17" s="11" t="s">
         <v>4</v>
       </c>
       <c r="F17" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="G17" s="10" t="s">
+      <c r="G17" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="H17" s="10" t="s">
+      <c r="H17" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="I17" s="8"/>
+      <c r="I17" s="9"/>
     </row>
     <row r="18" spans="2:9">
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="8"/>
-      <c r="I18" s="7" t="s">
+      <c r="B18" s="9"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="8" t="s">
         <v>9</v>
       </c>
     </row>
@@ -2161,12 +2188,12 @@
     </row>
   </sheetData>
   <hyperlinks>
+    <hyperlink ref="C25" r:id="rId1" display="qa@demo.cloudnowtech.com"/>
+    <hyperlink ref="C21" r:id="rId1" display="qa@demo.cloudnowtech.com"/>
+    <hyperlink ref="C17" r:id="rId1" display="qa@demo.cloudnowtech.com"/>
+    <hyperlink ref="C12" r:id="rId1" display="qa@demo.cloudnowtech.com"/>
+    <hyperlink ref="G7" r:id="rId2" display="test50@demo.cloudnowtech.com"/>
     <hyperlink ref="C7" r:id="rId1" display="qa@demo.cloudnowtech.com"/>
-    <hyperlink ref="G7" r:id="rId2" display="test50@demo.cloudnowtech.com"/>
-    <hyperlink ref="C12" r:id="rId1" display="qa@demo.cloudnowtech.com"/>
-    <hyperlink ref="C17" r:id="rId1" display="qa@demo.cloudnowtech.com"/>
-    <hyperlink ref="C21" r:id="rId1" display="qa@demo.cloudnowtech.com"/>
-    <hyperlink ref="C25" r:id="rId1" display="qa@demo.cloudnowtech.com"/>
   </hyperlinks>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
@@ -2180,13 +2207,13 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="B7:G31"/>
+  <dimension ref="B7:H35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="H37" sqref="H37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="7"/>
   <cols>
     <col min="2" max="2" width="34.8571428571429" customWidth="1"/>
     <col min="3" max="3" width="30.4285714285714" customWidth="1"/>
@@ -2194,6 +2221,7 @@
     <col min="5" max="5" width="17.4285714285714" customWidth="1"/>
     <col min="6" max="6" width="16.8571428571429" customWidth="1"/>
     <col min="7" max="7" width="34.8571428571429" customWidth="1"/>
+    <col min="8" max="8" width="31.7142857142857" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="7" spans="2:7">
@@ -2460,14 +2488,67 @@
         <v>67</v>
       </c>
     </row>
+    <row r="33" spans="2:8">
+      <c r="B33" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="H33" s="2"/>
+    </row>
+    <row r="34" spans="2:8">
+      <c r="B34" s="2"/>
+      <c r="C34" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G34" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="H34" s="2"/>
+    </row>
+    <row r="35" spans="2:8">
+      <c r="B35" s="5"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="5"/>
+      <c r="F35" s="5"/>
+      <c r="G35" s="5"/>
+      <c r="H35" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C8" r:id="rId1" display="qa@demo.cloudnowtech.com"/>
-    <hyperlink ref="C26" r:id="rId1" display="qa@demo.cloudnowtech.com"/>
-    <hyperlink ref="C12" r:id="rId1" display="qa@demo.cloudnowtech.com"/>
-    <hyperlink ref="C30" r:id="rId1" display="qa@demo.cloudnowtech.com"/>
-    <hyperlink ref="C16" r:id="rId1" display="qa@demo.cloudnowtech.com"/>
-    <hyperlink ref="C20" r:id="rId1" display="qa@demo.cloudnowtech.com"/>
+    <hyperlink ref="G34" r:id="rId1" display="test031@demo.cloudnowtech.com " tooltip="mailto:test031@demo.cloudnowtech.com "/>
+    <hyperlink ref="C34" r:id="rId2" display="qa@demo.cloudnowtech.com"/>
+    <hyperlink ref="C20" r:id="rId2" display="qa@demo.cloudnowtech.com"/>
+    <hyperlink ref="C16" r:id="rId2" display="qa@demo.cloudnowtech.com"/>
+    <hyperlink ref="C30" r:id="rId2" display="qa@demo.cloudnowtech.com"/>
+    <hyperlink ref="C12" r:id="rId2" display="qa@demo.cloudnowtech.com"/>
+    <hyperlink ref="C26" r:id="rId2" display="qa@demo.cloudnowtech.com"/>
+    <hyperlink ref="C8" r:id="rId2" display="qa@demo.cloudnowtech.com"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>

<commit_message>
Extent Report and log4j
</commit_message>
<xml_diff>
--- a/src/test/resources/input/Login.xlsx
+++ b/src/test/resources/input/Login.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12640" tabRatio="500" firstSheet="3" activeTab="6"/>
+    <workbookView windowWidth="28620" windowHeight="12640" tabRatio="500" firstSheet="3" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -244,11 +244,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="16">
     <font>
@@ -260,8 +260,29 @@
     </font>
     <font>
       <sz val="10"/>
+      <color indexed="23"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <name val="Arial"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="55"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <u/>
@@ -272,17 +293,8 @@
       <charset val="1"/>
     </font>
     <font>
-      <b/>
-      <sz val="24"/>
-      <color indexed="50"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
       <sz val="10"/>
-      <color indexed="50"/>
+      <color indexed="9"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -303,22 +315,17 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="12"/>
+      <b/>
+      <sz val="10"/>
       <color indexed="50"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color indexed="55"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color indexed="23"/>
+      <b/>
+      <sz val="24"/>
+      <color indexed="50"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -331,16 +338,17 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color indexed="9"/>
+      <sz val="12"/>
+      <color indexed="50"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color indexed="11"/>
-      <name val="Calibri"/>
+      <u/>
+      <sz val="11"/>
+      <color indexed="12"/>
+      <name val="宋体"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -349,13 +357,6 @@
       <sz val="10"/>
       <color indexed="23"/>
       <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color indexed="12"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -388,13 +389,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor indexed="50"/>
+        <bgColor indexed="50"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="18"/>
+        <bgColor indexed="23"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="34"/>
+        <bgColor indexed="19"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor indexed="23"/>
         <bgColor indexed="39"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="18"/>
+        <fgColor indexed="39"/>
         <bgColor indexed="23"/>
       </patternFill>
     </fill>
@@ -406,26 +425,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="39"/>
-        <bgColor indexed="23"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="34"/>
-        <bgColor indexed="19"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor indexed="52"/>
         <bgColor indexed="8"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="50"/>
-        <bgColor indexed="50"/>
       </patternFill>
     </fill>
   </fills>
@@ -487,86 +488,86 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyBorder="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyBorder="0" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="3" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyBorder="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyBorder="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyBorder="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyBorder="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyBorder="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyBorder="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyBorder="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyBorder="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyBorder="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyBorder="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyBorder="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyBorder="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyBorder="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyBorder="0" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyBorder="0" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyBorder="0" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyBorder="0" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyBorder="0" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="top"/>
     </xf>
@@ -585,10 +586,10 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="25" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="25" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="15" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="15" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -597,10 +598,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="15" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="15" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="25" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1054,7 +1058,7 @@
   <dimension ref="B6:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="4"/>
@@ -1178,14 +1182,14 @@
   <dimension ref="B9:J28"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="3.85714285714286" customWidth="1"/>
-    <col min="2" max="2" width="31.4190476190476" customWidth="1"/>
-    <col min="3" max="3" width="26.7904761904762" customWidth="1"/>
+    <col min="2" max="2" width="32.8571428571429" customWidth="1"/>
+    <col min="3" max="3" width="34.1428571428571" customWidth="1"/>
     <col min="4" max="4" width="17.5333333333333" customWidth="1"/>
     <col min="5" max="6" width="19.5142857142857" customWidth="1"/>
     <col min="7" max="7" width="19.0666666666667" customWidth="1"/>
@@ -1194,48 +1198,48 @@
   </cols>
   <sheetData>
     <row r="9" spans="2:10">
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="E9" s="8" t="s">
+      <c r="C9" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F9" s="8" t="s">
+      <c r="F9" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G9" s="8" t="s">
+      <c r="G9" s="1" t="s">
         <v>12</v>
       </c>
       <c r="H9" s="9"/>
-      <c r="I9" s="16"/>
-      <c r="J9" s="17"/>
+      <c r="I9" s="17"/>
+      <c r="J9" s="18"/>
     </row>
     <row r="10" spans="2:10">
-      <c r="B10" s="9"/>
-      <c r="C10" s="10" t="s">
+      <c r="B10" s="2"/>
+      <c r="C10" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D10" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="E10" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="F10" s="11" t="s">
+      <c r="D10" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F10" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G10" s="11" t="s">
+      <c r="G10" s="2" t="s">
         <v>13</v>
       </c>
       <c r="H10" s="9"/>
-      <c r="I10" s="17"/>
-      <c r="J10" s="17"/>
+      <c r="I10" s="18"/>
+      <c r="J10" s="18"/>
     </row>
     <row r="11" spans="2:10">
       <c r="B11" s="9"/>
@@ -1247,12 +1251,12 @@
       <c r="H11" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="I11" s="17"/>
-      <c r="J11" s="17"/>
+      <c r="I11" s="18"/>
+      <c r="J11" s="18"/>
     </row>
     <row r="12" spans="9:10">
-      <c r="I12" s="17"/>
-      <c r="J12" s="17"/>
+      <c r="I12" s="18"/>
+      <c r="J12" s="18"/>
     </row>
     <row r="13" spans="2:10">
       <c r="B13" s="8" t="s">
@@ -1274,8 +1278,8 @@
         <v>12</v>
       </c>
       <c r="H13" s="9"/>
-      <c r="I13" s="16"/>
-      <c r="J13" s="16"/>
+      <c r="I13" s="17"/>
+      <c r="J13" s="17"/>
     </row>
     <row r="14" spans="2:8">
       <c r="B14" s="9"/>
@@ -1410,7 +1414,7 @@
       </c>
     </row>
     <row r="26" ht="30" spans="2:8">
-      <c r="B26" s="15" t="s">
+      <c r="B26" s="16" t="s">
         <v>18</v>
       </c>
       <c r="C26" s="8" t="s">
@@ -1456,7 +1460,7 @@
       <c r="E28" s="9"/>
       <c r="F28" s="9"/>
       <c r="G28" s="9"/>
-      <c r="H28" s="15" t="s">
+      <c r="H28" s="16" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1517,7 +1521,7 @@
       <c r="E8" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F8" s="14" t="s">
+      <c r="F8" s="15" t="s">
         <v>21</v>
       </c>
       <c r="G8" s="2"/>
@@ -1800,31 +1804,31 @@
       <c r="H7" s="9"/>
     </row>
     <row r="8" spans="2:8">
-      <c r="B8" s="12"/>
+      <c r="B8" s="13"/>
       <c r="C8" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="12" t="s">
+      <c r="D8" s="13" t="s">
         <v>4</v>
       </c>
       <c r="E8" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="F8" s="12" t="s">
+      <c r="F8" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="G8" s="12" t="s">
+      <c r="G8" s="13" t="s">
         <v>4</v>
       </c>
       <c r="H8" s="9"/>
     </row>
     <row r="9" spans="2:8">
-      <c r="B9" s="13"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
+      <c r="B9" s="14"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
       <c r="H9" s="8" t="s">
         <v>33</v>
       </c>
@@ -1858,7 +1862,7 @@
       <c r="C13" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="D13" s="12" t="s">
+      <c r="D13" s="13" t="s">
         <v>4</v>
       </c>
       <c r="E13" s="11" t="s">
@@ -1870,7 +1874,7 @@
       <c r="G13" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="H13" s="12" t="s">
+      <c r="H13" s="13" t="s">
         <v>4</v>
       </c>
       <c r="I13" s="9"/>
@@ -1907,8 +1911,8 @@
   <sheetPr/>
   <dimension ref="B6:I26"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:H8"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1917,9 +1921,10 @@
     <col min="2" max="2" width="22.3714285714286" customWidth="1"/>
     <col min="3" max="3" width="30.2571428571429" customWidth="1"/>
     <col min="4" max="4" width="18.7428571428571" customWidth="1"/>
-    <col min="5" max="6" width="20.8285714285714" customWidth="1"/>
+    <col min="5" max="5" width="20.8285714285714" customWidth="1"/>
+    <col min="6" max="6" width="35.2857142857143" customWidth="1"/>
     <col min="7" max="7" width="32.9523809523809" customWidth="1"/>
-    <col min="8" max="8" width="22.3714285714286" customWidth="1"/>
+    <col min="8" max="8" width="27.5714285714286" customWidth="1"/>
     <col min="9" max="9" width="20.4" customWidth="1"/>
     <col min="10" max="1025" width="9.14285714285714" customWidth="1"/>
   </cols>
@@ -2061,7 +2066,7 @@
       <c r="E17" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="F17" s="4" t="s">
+      <c r="F17" s="12" t="s">
         <v>51</v>
       </c>
       <c r="G17" s="11" t="s">
@@ -2188,12 +2193,13 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C25" r:id="rId1" display="qa@demo.cloudnowtech.com"/>
-    <hyperlink ref="C21" r:id="rId1" display="qa@demo.cloudnowtech.com"/>
-    <hyperlink ref="C17" r:id="rId1" display="qa@demo.cloudnowtech.com"/>
-    <hyperlink ref="C12" r:id="rId1" display="qa@demo.cloudnowtech.com"/>
-    <hyperlink ref="G7" r:id="rId2" display="test50@demo.cloudnowtech.com"/>
-    <hyperlink ref="C7" r:id="rId1" display="qa@demo.cloudnowtech.com"/>
+    <hyperlink ref="F17" r:id="rId1" display="test001@demo.cloudnowtech.com"/>
+    <hyperlink ref="C25" r:id="rId2" display="qa@demo.cloudnowtech.com"/>
+    <hyperlink ref="C21" r:id="rId2" display="qa@demo.cloudnowtech.com"/>
+    <hyperlink ref="C17" r:id="rId2" display="qa@demo.cloudnowtech.com"/>
+    <hyperlink ref="C12" r:id="rId2" display="qa@demo.cloudnowtech.com"/>
+    <hyperlink ref="G7" r:id="rId3" display="test50@demo.cloudnowtech.com"/>
+    <hyperlink ref="C7" r:id="rId2" display="qa@demo.cloudnowtech.com"/>
   </hyperlinks>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
@@ -2209,7 +2215,7 @@
   <sheetPr/>
   <dimension ref="B7:H35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="H37" sqref="H37"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Sync ou via Gsuite
</commit_message>
<xml_diff>
--- a/src/test/resources/input/Login.xlsx
+++ b/src/test/resources/input/Login.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="28620" windowHeight="12640" tabRatio="500" firstSheet="3" activeTab="5"/>
+    <workbookView windowWidth="28620" windowHeight="12640" tabRatio="500" firstSheet="3" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -244,11 +244,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="16">
     <font>
@@ -260,59 +260,8 @@
     </font>
     <font>
       <sz val="10"/>
-      <color indexed="23"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
       <name val="Arial"/>
       <charset val="134"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color indexed="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color indexed="55"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color indexed="31"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color indexed="9"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color indexed="52"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="10"/>
-      <color indexed="15"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b/>
@@ -331,8 +280,38 @@
       <charset val="1"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color indexed="31"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="55"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <sz val="18"/>
       <color indexed="50"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color indexed="12"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="52"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -345,10 +324,31 @@
       <charset val="1"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color indexed="12"/>
-      <name val="宋体"/>
+      <sz val="10"/>
+      <color indexed="23"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color indexed="15"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="9"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -389,26 +389,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="50"/>
-        <bgColor indexed="50"/>
+        <fgColor indexed="23"/>
+        <bgColor indexed="39"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="18"/>
         <bgColor indexed="23"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="34"/>
-        <bgColor indexed="19"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="23"/>
-        <bgColor indexed="39"/>
       </patternFill>
     </fill>
     <fill>
@@ -425,8 +413,20 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor indexed="34"/>
+        <bgColor indexed="19"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor indexed="52"/>
         <bgColor indexed="8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="50"/>
+        <bgColor indexed="50"/>
       </patternFill>
     </fill>
   </fills>
@@ -488,82 +488,82 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyBorder="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyBorder="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyBorder="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyBorder="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyBorder="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyBorder="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyBorder="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyBorder="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyBorder="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyBorder="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyBorder="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyBorder="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyBorder="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyBorder="0" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyBorder="0" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyBorder="0" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyBorder="0" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyBorder="0" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
   </cellStyleXfs>
@@ -586,10 +586,10 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="25" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="25" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="15" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="15" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -598,13 +598,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="15" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="15" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="25" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="25" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1764,8 +1764,8 @@
   <sheetPr/>
   <dimension ref="B7:I14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1911,8 +1911,8 @@
   <sheetPr/>
   <dimension ref="B6:I26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E45" sqref="E45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -2216,7 +2216,7 @@
   <dimension ref="B7:H35"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="H37" sqref="H37"/>
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="7"/>

</xml_diff>

<commit_message>
Site blocking Based on OU
</commit_message>
<xml_diff>
--- a/src/test/resources/input/Login.xlsx
+++ b/src/test/resources/input/Login.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="28620" windowHeight="12640" tabRatio="500" firstSheet="3" activeTab="4"/>
+    <workbookView windowWidth="28620" windowHeight="12500" tabRatio="500" firstSheet="3" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81">
   <si>
     <t>Valid_LoginDetails</t>
   </si>
@@ -56,18 +56,27 @@
     <t>Oldpassword</t>
   </si>
   <si>
+    <t>newemail</t>
+  </si>
+  <si>
     <t>Newpassword</t>
   </si>
   <si>
     <t>Confnewpassword</t>
   </si>
   <si>
+    <t>test50@demo.cloudnowtech.com</t>
+  </si>
+  <si>
+    <t>password4</t>
+  </si>
+  <si>
+    <t>ChangeNewPWDtoOldPWD</t>
+  </si>
+  <si>
     <t>password2</t>
   </si>
   <si>
-    <t>ChangeNewPWDtoOldPWD</t>
-  </si>
-  <si>
     <t>InvalidConfirmpassword_Details</t>
   </si>
   <si>
@@ -122,6 +131,33 @@
     <t>twitter1.com</t>
   </si>
   <si>
+    <t>SiteUrlForParentOU</t>
+  </si>
+  <si>
+    <t>proxyemail</t>
+  </si>
+  <si>
+    <t>proxypassword</t>
+  </si>
+  <si>
+    <t>ParentOU</t>
+  </si>
+  <si>
+    <t>test004@demo.cloudnowtech.com</t>
+  </si>
+  <si>
+    <t>DemoFN</t>
+  </si>
+  <si>
+    <t>SiteUrlForChildOU</t>
+  </si>
+  <si>
+    <t>test005@demo.cloudnowtech.com</t>
+  </si>
+  <si>
+    <t>www.flipkart.com</t>
+  </si>
+  <si>
     <t>AddSingleUser</t>
   </si>
   <si>
@@ -161,15 +197,9 @@
     <t>NewEmail</t>
   </si>
   <si>
-    <t>DemoFN</t>
-  </si>
-  <si>
     <t>DemoLN</t>
   </si>
   <si>
-    <t>test50@demo.cloudnowtech.com</t>
-  </si>
-  <si>
     <t>InvalidEmailFormat</t>
   </si>
   <si>
@@ -197,9 +227,6 @@
     <t>NewOu</t>
   </si>
   <si>
-    <t>ParentOU</t>
-  </si>
-  <si>
     <t>CNT</t>
   </si>
   <si>
@@ -215,7 +242,7 @@
     <t>DuplicateOUwithdifferntParentOU</t>
   </si>
   <si>
-    <t>Google</t>
+    <t>TestTest</t>
   </si>
   <si>
     <t>EditOU</t>
@@ -264,22 +291,6 @@
       <charset val="134"/>
     </font>
     <font>
-      <b/>
-      <sz val="10"/>
-      <color indexed="50"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="24"/>
-      <color indexed="50"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color indexed="31"/>
@@ -289,7 +300,30 @@
     </font>
     <font>
       <sz val="10"/>
+      <color indexed="23"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color indexed="55"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color indexed="50"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color indexed="15"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -310,8 +344,9 @@
       <charset val="1"/>
     </font>
     <font>
+      <b/>
       <sz val="10"/>
-      <color indexed="52"/>
+      <color indexed="23"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -324,16 +359,9 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color indexed="23"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="10"/>
-      <color indexed="15"/>
+      <b/>
+      <sz val="24"/>
+      <color indexed="50"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -353,9 +381,8 @@
       <charset val="1"/>
     </font>
     <font>
-      <b/>
       <sz val="10"/>
-      <color indexed="23"/>
+      <color indexed="52"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -389,8 +416,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="23"/>
-        <bgColor indexed="39"/>
+        <fgColor indexed="50"/>
+        <bgColor indexed="50"/>
       </patternFill>
     </fill>
     <fill>
@@ -401,8 +428,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="39"/>
-        <bgColor indexed="23"/>
+        <fgColor indexed="23"/>
+        <bgColor indexed="39"/>
       </patternFill>
     </fill>
     <fill>
@@ -413,20 +440,20 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor indexed="52"/>
+        <bgColor indexed="8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor indexed="34"/>
         <bgColor indexed="19"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="52"/>
-        <bgColor indexed="8"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="50"/>
-        <bgColor indexed="50"/>
+        <fgColor indexed="39"/>
+        <bgColor indexed="23"/>
       </patternFill>
     </fill>
   </fills>
@@ -506,7 +533,7 @@
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyBorder="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -515,59 +542,59 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyBorder="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyBorder="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyBorder="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyBorder="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyBorder="0" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyBorder="0" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyBorder="0" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyBorder="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyBorder="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyBorder="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyBorder="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyBorder="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyBorder="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyBorder="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyBorder="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="top"/>
     </xf>
@@ -586,10 +613,10 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="25" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="25" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="15" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="16" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -598,13 +625,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="15" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="16" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="25" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="25" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -613,16 +640,19 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -639,11 +669,11 @@
     <cellStyle name="Currency[0]" xfId="9" builtinId="7"/>
     <cellStyle name="Heading" xfId="10"/>
     <cellStyle name="Heading 1" xfId="11"/>
-    <cellStyle name="Note" xfId="12"/>
-    <cellStyle name="Heading 2" xfId="13"/>
+    <cellStyle name="Heading 2" xfId="12"/>
+    <cellStyle name="Note" xfId="13"/>
     <cellStyle name="Footnote" xfId="14"/>
-    <cellStyle name="*unknown*" xfId="15"/>
-    <cellStyle name="Status" xfId="16"/>
+    <cellStyle name="Status" xfId="15"/>
+    <cellStyle name="*unknown*" xfId="16"/>
     <cellStyle name="Good" xfId="17"/>
     <cellStyle name="Neutral" xfId="18"/>
     <cellStyle name="Bad" xfId="19"/>
@@ -1166,9 +1196,9 @@
     </row>
   </sheetData>
   <hyperlinks>
+    <hyperlink ref="C7" r:id="rId1" display="qa@demo.cloudnowtech.com"/>
+    <hyperlink ref="C13" r:id="rId2" display="invalidEmail@demo.cloudnowtech.com"/>
     <hyperlink ref="C19" r:id="rId1" display="qa@demo.cloudnowtech.com"/>
-    <hyperlink ref="C13" r:id="rId2" display="invalidEmail@demo.cloudnowtech.com"/>
-    <hyperlink ref="C7" r:id="rId1" display="qa@demo.cloudnowtech.com"/>
   </hyperlinks>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.510416666666667" footer="0.510416666666667"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
@@ -1182,7 +1212,7 @@
   <dimension ref="B9:J28"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+      <selection activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1191,10 +1221,12 @@
     <col min="2" max="2" width="32.8571428571429" customWidth="1"/>
     <col min="3" max="3" width="34.1428571428571" customWidth="1"/>
     <col min="4" max="4" width="17.5333333333333" customWidth="1"/>
-    <col min="5" max="6" width="19.5142857142857" customWidth="1"/>
+    <col min="5" max="5" width="19.5142857142857" customWidth="1"/>
+    <col min="6" max="6" width="34.1428571428571" customWidth="1"/>
     <col min="7" max="7" width="19.0666666666667" customWidth="1"/>
     <col min="8" max="8" width="30.9809523809524" customWidth="1"/>
-    <col min="9" max="1025" width="8.53333333333333" customWidth="1"/>
+    <col min="9" max="9" width="24.7142857142857" customWidth="1"/>
+    <col min="10" max="1025" width="8.53333333333333" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="9" spans="2:10">
@@ -1210,14 +1242,16 @@
       <c r="E9" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="F9" s="8" t="s">
         <v>11</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H9" s="9"/>
-      <c r="I9" s="17"/>
+      <c r="H9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I9" s="9"/>
       <c r="J9" s="18"/>
     </row>
     <row r="10" spans="2:10">
@@ -1231,14 +1265,16 @@
       <c r="E10" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F10" s="2" t="s">
-        <v>13</v>
+      <c r="F10" s="4" t="s">
+        <v>14</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H10" s="9"/>
-      <c r="I10" s="18"/>
+        <v>15</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I10" s="9"/>
       <c r="J10" s="18"/>
     </row>
     <row r="11" spans="2:10">
@@ -1246,12 +1282,11 @@
       <c r="C11" s="9"/>
       <c r="D11" s="9"/>
       <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
       <c r="G11" s="9"/>
-      <c r="H11" s="8" t="s">
+      <c r="H11" s="9"/>
+      <c r="I11" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="I11" s="18"/>
       <c r="J11" s="18"/>
     </row>
     <row r="12" spans="9:10">
@@ -1260,7 +1295,7 @@
     </row>
     <row r="13" spans="2:10">
       <c r="B13" s="8" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C13" s="8" t="s">
         <v>1</v>
@@ -1272,14 +1307,14 @@
         <v>10</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G13" s="8" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H13" s="9"/>
-      <c r="I13" s="17"/>
-      <c r="J13" s="17"/>
+      <c r="I13" s="19"/>
+      <c r="J13" s="19"/>
     </row>
     <row r="14" spans="2:8">
       <c r="B14" s="9"/>
@@ -1287,10 +1322,10 @@
         <v>3</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F14" s="11" t="s">
         <v>4</v>
@@ -1308,12 +1343,12 @@
       <c r="F15" s="9"/>
       <c r="G15" s="9"/>
       <c r="H15" s="8" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="2:8">
       <c r="B18" s="8" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C18" s="8" t="s">
         <v>1</v>
@@ -1325,10 +1360,10 @@
         <v>10</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G18" s="8" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H18" s="9"/>
     </row>
@@ -1344,7 +1379,7 @@
         <v>4</v>
       </c>
       <c r="F19" s="11" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="G19" s="11" t="s">
         <v>2</v>
@@ -1359,12 +1394,12 @@
       <c r="F20" s="9"/>
       <c r="G20" s="9"/>
       <c r="H20" s="8" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="22" spans="2:8">
       <c r="B22" s="8" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C22" s="8" t="s">
         <v>1</v>
@@ -1376,10 +1411,10 @@
         <v>10</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G22" s="8" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H22" s="9"/>
     </row>
@@ -1392,13 +1427,13 @@
         <v>4</v>
       </c>
       <c r="E23" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="F23" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="F23" s="11" t="s">
-        <v>13</v>
-      </c>
       <c r="G23" s="11" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="H23" s="9"/>
     </row>
@@ -1410,12 +1445,12 @@
       <c r="F24" s="9"/>
       <c r="G24" s="9"/>
       <c r="H24" s="8" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="26" ht="30" spans="2:8">
-      <c r="B26" s="16" t="s">
-        <v>18</v>
+      <c r="B26" s="17" t="s">
+        <v>21</v>
       </c>
       <c r="C26" s="8" t="s">
         <v>1</v>
@@ -1427,10 +1462,10 @@
         <v>10</v>
       </c>
       <c r="F26" s="8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G26" s="8" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H26" s="9"/>
     </row>
@@ -1443,13 +1478,13 @@
         <v>4</v>
       </c>
       <c r="E27" s="11" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="F27" s="11" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="G27" s="11" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="H27" s="9"/>
     </row>
@@ -1460,17 +1495,18 @@
       <c r="E28" s="9"/>
       <c r="F28" s="9"/>
       <c r="G28" s="9"/>
-      <c r="H28" s="16" t="s">
-        <v>18</v>
+      <c r="H28" s="17" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C27" r:id="rId1" display="qa@demo.cloudnowtech.com"/>
-    <hyperlink ref="C23" r:id="rId1" display="qa@demo.cloudnowtech.com"/>
-    <hyperlink ref="C19" r:id="rId1" display="qa@demo.cloudnowtech.com"/>
-    <hyperlink ref="C14" r:id="rId1" display="qa@demo.cloudnowtech.com"/>
-    <hyperlink ref="C10" r:id="rId1" display="qa@demo.cloudnowtech.com"/>
+    <hyperlink ref="F10" r:id="rId1" display="test50@demo.cloudnowtech.com" tooltip="mailto:test50@demo.cloudnowtech.com"/>
+    <hyperlink ref="C10" r:id="rId2" display="qa@demo.cloudnowtech.com"/>
+    <hyperlink ref="C14" r:id="rId2" display="qa@demo.cloudnowtech.com"/>
+    <hyperlink ref="C19" r:id="rId2" display="qa@demo.cloudnowtech.com"/>
+    <hyperlink ref="C23" r:id="rId2" display="qa@demo.cloudnowtech.com"/>
+    <hyperlink ref="C27" r:id="rId2" display="qa@demo.cloudnowtech.com"/>
   </hyperlinks>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.510416666666667" footer="0.510416666666667"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
@@ -1509,7 +1545,7 @@
         <v>2</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="G7" s="2"/>
     </row>
@@ -1521,8 +1557,8 @@
       <c r="E8" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F8" s="15" t="s">
-        <v>21</v>
+      <c r="F8" s="16" t="s">
+        <v>24</v>
       </c>
       <c r="G8" s="2"/>
     </row>
@@ -1537,8 +1573,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F8" r:id="rId1" display="qacsv@demo.cloudnowtech.com"/>
-    <hyperlink ref="D8" r:id="rId2" display="qa@demo.cloudnowtech.com"/>
+    <hyperlink ref="D8" r:id="rId1" display="qa@demo.cloudnowtech.com"/>
+    <hyperlink ref="F8" r:id="rId2" display="qacsv@demo.cloudnowtech.com"/>
   </hyperlinks>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.510416666666667" footer="0.510416666666667"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
@@ -1549,22 +1585,24 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="B5:G23"/>
+  <dimension ref="B5:J32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="4.73333333333333" customWidth="1"/>
     <col min="2" max="2" width="25.3619047619048" customWidth="1"/>
-    <col min="3" max="3" width="27.0095238095238" customWidth="1"/>
+    <col min="3" max="3" width="30.4285714285714" customWidth="1"/>
     <col min="4" max="4" width="14.7714285714286" customWidth="1"/>
     <col min="5" max="5" width="37.0380952380952" customWidth="1"/>
     <col min="6" max="6" width="21.0380952380952" customWidth="1"/>
     <col min="7" max="7" width="25.7904761904762" customWidth="1"/>
-    <col min="8" max="1025" width="9.14285714285714" customWidth="1"/>
+    <col min="8" max="9" width="15.5714285714286" customWidth="1"/>
+    <col min="10" max="10" width="18.7142857142857" customWidth="1"/>
+    <col min="11" max="1026" width="9.14285714285714" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="5" spans="2:7">
@@ -1578,10 +1616,10 @@
         <v>2</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="G5" s="5"/>
     </row>
@@ -1594,10 +1632,10 @@
         <v>4</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="G6" s="2"/>
     </row>
@@ -1613,19 +1651,19 @@
     </row>
     <row r="9" spans="2:7">
       <c r="B9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>23</v>
       </c>
       <c r="G9" s="5"/>
     </row>
@@ -1638,10 +1676,10 @@
         <v>4</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="G10" s="2"/>
     </row>
@@ -1652,12 +1690,12 @@
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
       <c r="G11" s="1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="2:6">
       <c r="B15" s="1" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>1</v>
@@ -1666,10 +1704,10 @@
         <v>2</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="16" spans="2:7">
@@ -1681,10 +1719,10 @@
         <v>4</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="G16" s="2"/>
     </row>
@@ -1695,12 +1733,12 @@
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
       <c r="G17" s="1" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="21" spans="2:6">
       <c r="B21" s="1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>1</v>
@@ -1709,10 +1747,10 @@
         <v>2</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="22" spans="2:7">
@@ -1724,10 +1762,10 @@
         <v>4</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="G22" s="2"/>
     </row>
@@ -1738,17 +1776,151 @@
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
       <c r="G23" s="1" t="s">
-        <v>31</v>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9">
+      <c r="B26" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I26" s="15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="27" spans="2:10">
+      <c r="B27" s="2"/>
+      <c r="C27" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G27" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I27" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="J27" s="2"/>
+    </row>
+    <row r="28" spans="2:10">
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
+      <c r="G28" s="5"/>
+      <c r="H28" s="5"/>
+      <c r="I28" s="5"/>
+      <c r="J28" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="30" spans="2:9">
+      <c r="B30" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I30" s="15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="31" spans="2:10">
+      <c r="B31" s="2"/>
+      <c r="C31" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E31" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G31" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I31" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="J31" s="2"/>
+    </row>
+    <row r="32" spans="2:10">
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
+      <c r="G32" s="5"/>
+      <c r="H32" s="5"/>
+      <c r="I32" s="5"/>
+      <c r="J32" s="1" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
+    <hyperlink ref="C6" r:id="rId1" display="qa@demo.cloudnowtech.com"/>
+    <hyperlink ref="E6" r:id="rId2" display="www.google.com" tooltip="http://www.google.com"/>
+    <hyperlink ref="C10" r:id="rId1" display="qa@demo.cloudnowtech.com"/>
+    <hyperlink ref="E10" r:id="rId3" display="www.yahoo.com"/>
+    <hyperlink ref="C16" r:id="rId1" display="qa@demo.cloudnowtech.com"/>
     <hyperlink ref="C22" r:id="rId1" display="qa@demo.cloudnowtech.com"/>
-    <hyperlink ref="C16" r:id="rId1" display="qa@demo.cloudnowtech.com"/>
-    <hyperlink ref="E10" r:id="rId2" display="www.yahoo.com"/>
-    <hyperlink ref="C10" r:id="rId1" display="qa@demo.cloudnowtech.com"/>
-    <hyperlink ref="E6" r:id="rId3" display="www.google.com"/>
-    <hyperlink ref="C6" r:id="rId1" display="qa@demo.cloudnowtech.com"/>
+    <hyperlink ref="C27" r:id="rId1" display="qa@demo.cloudnowtech.com"/>
+    <hyperlink ref="E27" r:id="rId4" display="test004@demo.cloudnowtech.com" tooltip="mailto:test004@demo.cloudnowtech.com"/>
+    <hyperlink ref="G27" r:id="rId5" display="www.yahoo.com"/>
+    <hyperlink ref="C31" r:id="rId1" display="qa@demo.cloudnowtech.com"/>
+    <hyperlink ref="E31" r:id="rId6" display="test005@demo.cloudnowtech.com" tooltip="mailto:test005@demo.cloudnowtech.com"/>
+    <hyperlink ref="G31" r:id="rId7" display="www.flipkart.com" tooltip="http://www.flipkart.com"/>
   </hyperlinks>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
@@ -1764,7 +1936,7 @@
   <sheetPr/>
   <dimension ref="B7:I14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
@@ -1784,7 +1956,7 @@
   <sheetData>
     <row r="7" spans="2:8">
       <c r="B7" s="8" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="C7" s="8" t="s">
         <v>1</v>
@@ -1793,13 +1965,13 @@
         <v>2</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H7" s="9"/>
     </row>
@@ -1812,10 +1984,10 @@
         <v>4</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="F8" s="13" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="G8" s="13" t="s">
         <v>4</v>
@@ -1830,12 +2002,12 @@
       <c r="F9" s="14"/>
       <c r="G9" s="14"/>
       <c r="H9" s="8" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="2:9">
       <c r="B12" s="8" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="C12" s="8" t="s">
         <v>1</v>
@@ -1844,16 +2016,16 @@
         <v>2</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="H12" s="8" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I12" s="9"/>
     </row>
@@ -1866,13 +2038,13 @@
         <v>4</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="F13" s="11" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="G13" s="11" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="H13" s="13" t="s">
         <v>4</v>
@@ -1888,14 +2060,14 @@
       <c r="G14" s="9"/>
       <c r="H14" s="9"/>
       <c r="I14" s="8" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E13" r:id="rId1" display="mathi.t@demo.cloudnowtech.com"/>
-    <hyperlink ref="C13" r:id="rId2" display="qa@demo.cloudnowtech.com"/>
-    <hyperlink ref="C8" r:id="rId2" display="qa@demo.cloudnowtech.com"/>
+    <hyperlink ref="C8" r:id="rId1" display="qa@demo.cloudnowtech.com"/>
+    <hyperlink ref="C13" r:id="rId1" display="qa@demo.cloudnowtech.com"/>
+    <hyperlink ref="E13" r:id="rId2" display="mathi.t@demo.cloudnowtech.com"/>
   </hyperlinks>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
@@ -1912,7 +2084,7 @@
   <dimension ref="B6:I26"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E45" sqref="E45"/>
+      <selection activeCell="F45" sqref="F45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1922,8 +2094,7 @@
     <col min="3" max="3" width="30.2571428571429" customWidth="1"/>
     <col min="4" max="4" width="18.7428571428571" customWidth="1"/>
     <col min="5" max="5" width="20.8285714285714" customWidth="1"/>
-    <col min="6" max="6" width="35.2857142857143" customWidth="1"/>
-    <col min="7" max="7" width="32.9523809523809" customWidth="1"/>
+    <col min="6" max="7" width="35.2857142857143" customWidth="1"/>
     <col min="8" max="8" width="27.5714285714286" customWidth="1"/>
     <col min="9" max="9" width="20.4" customWidth="1"/>
     <col min="10" max="1025" width="9.14285714285714" customWidth="1"/>
@@ -1931,7 +2102,7 @@
   <sheetData>
     <row r="6" spans="2:8">
       <c r="B6" s="1" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>1</v>
@@ -1940,13 +2111,13 @@
         <v>2</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="H6" s="2"/>
     </row>
@@ -1959,13 +2130,13 @@
         <v>4</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="H7" s="2"/>
     </row>
@@ -1977,12 +2148,12 @@
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
       <c r="H8" s="1" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="2:8">
       <c r="B11" s="1" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>1</v>
@@ -1991,13 +2162,13 @@
         <v>2</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="H11" s="5"/>
     </row>
@@ -2010,13 +2181,13 @@
         <v>4</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="H12" s="2"/>
     </row>
@@ -2028,7 +2199,7 @@
       <c r="F13" s="5"/>
       <c r="G13" s="5"/>
       <c r="H13" s="1" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
     </row>
     <row r="16" spans="2:9">
@@ -2045,13 +2216,13 @@
         <v>10</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="G16" s="8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H16" s="8" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I16" s="9"/>
     </row>
@@ -2067,13 +2238,13 @@
         <v>4</v>
       </c>
       <c r="F17" s="12" t="s">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="G17" s="11" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="H17" s="11" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="I17" s="9"/>
     </row>
@@ -2091,7 +2262,7 @@
     </row>
     <row r="20" spans="2:8">
       <c r="B20" s="1" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>1</v>
@@ -2100,13 +2271,13 @@
         <v>2</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="H20" s="2"/>
     </row>
@@ -2119,13 +2290,13 @@
         <v>4</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="H21" s="2"/>
     </row>
@@ -2137,12 +2308,12 @@
       <c r="F22" s="5"/>
       <c r="G22" s="5"/>
       <c r="H22" s="1" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
     </row>
     <row r="24" spans="2:8">
       <c r="B24" s="1" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>1</v>
@@ -2151,13 +2322,13 @@
         <v>2</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="H24" s="2"/>
     </row>
@@ -2170,13 +2341,13 @@
         <v>4</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="H25" s="2"/>
     </row>
@@ -2188,18 +2359,18 @@
       <c r="F26" s="5"/>
       <c r="G26" s="5"/>
       <c r="H26" s="1" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F17" r:id="rId1" display="test001@demo.cloudnowtech.com"/>
-    <hyperlink ref="C25" r:id="rId2" display="qa@demo.cloudnowtech.com"/>
-    <hyperlink ref="C21" r:id="rId2" display="qa@demo.cloudnowtech.com"/>
-    <hyperlink ref="C17" r:id="rId2" display="qa@demo.cloudnowtech.com"/>
-    <hyperlink ref="C12" r:id="rId2" display="qa@demo.cloudnowtech.com"/>
-    <hyperlink ref="G7" r:id="rId3" display="test50@demo.cloudnowtech.com"/>
-    <hyperlink ref="C7" r:id="rId2" display="qa@demo.cloudnowtech.com"/>
+    <hyperlink ref="C7" r:id="rId1" display="qa@demo.cloudnowtech.com"/>
+    <hyperlink ref="G7" r:id="rId2" display="test50@demo.cloudnowtech.com" tooltip="mailto:test50@demo.cloudnowtech.com"/>
+    <hyperlink ref="C12" r:id="rId1" display="qa@demo.cloudnowtech.com"/>
+    <hyperlink ref="C17" r:id="rId1" display="qa@demo.cloudnowtech.com"/>
+    <hyperlink ref="C21" r:id="rId1" display="qa@demo.cloudnowtech.com"/>
+    <hyperlink ref="C25" r:id="rId1" display="qa@demo.cloudnowtech.com"/>
+    <hyperlink ref="F17" r:id="rId3" display="test001@demo.cloudnowtech.com"/>
   </hyperlinks>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
@@ -2216,7 +2387,7 @@
   <dimension ref="B7:H35"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="7"/>
@@ -2232,7 +2403,7 @@
   <sheetData>
     <row r="7" spans="2:7">
       <c r="B7" s="1" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>1</v>
@@ -2241,10 +2412,10 @@
         <v>2</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>58</v>
+        <v>39</v>
       </c>
       <c r="G7" s="2"/>
     </row>
@@ -2257,10 +2428,10 @@
         <v>4</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="G8" s="2"/>
     </row>
@@ -2271,12 +2442,12 @@
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
       <c r="G9" s="1" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
     </row>
     <row r="11" spans="2:7">
       <c r="B11" s="1" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>1</v>
@@ -2285,10 +2456,10 @@
         <v>2</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>58</v>
+        <v>39</v>
       </c>
       <c r="G11" s="2"/>
     </row>
@@ -2301,10 +2472,10 @@
         <v>4</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="G12" s="2"/>
     </row>
@@ -2315,12 +2486,12 @@
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
       <c r="G13" s="1" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
     </row>
     <row r="15" spans="2:7">
       <c r="B15" s="1" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>1</v>
@@ -2329,10 +2500,10 @@
         <v>2</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>58</v>
+        <v>39</v>
       </c>
       <c r="G15" s="2"/>
     </row>
@@ -2345,10 +2516,10 @@
         <v>4</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="G16" s="2"/>
     </row>
@@ -2359,12 +2530,12 @@
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
       <c r="G17" s="1" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
     </row>
     <row r="19" spans="2:7">
       <c r="B19" s="1" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>1</v>
@@ -2373,10 +2544,10 @@
         <v>2</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>58</v>
+        <v>39</v>
       </c>
       <c r="G19" s="2"/>
     </row>
@@ -2389,10 +2560,10 @@
         <v>4</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="G20" s="2"/>
     </row>
@@ -2403,12 +2574,12 @@
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
       <c r="G21" s="1" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
     </row>
     <row r="25" spans="2:7">
       <c r="B25" s="1" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>1</v>
@@ -2417,10 +2588,10 @@
         <v>2</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>58</v>
+        <v>39</v>
       </c>
       <c r="G25" s="2"/>
     </row>
@@ -2433,10 +2604,10 @@
         <v>4</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="G26" s="2"/>
     </row>
@@ -2447,24 +2618,24 @@
       <c r="E27" s="5"/>
       <c r="F27" s="5"/>
       <c r="G27" s="1" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
     </row>
     <row r="29" spans="2:7">
       <c r="B29" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E29" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C29" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>57</v>
-      </c>
       <c r="F29" s="1" t="s">
-        <v>58</v>
+        <v>39</v>
       </c>
       <c r="G29" s="2"/>
     </row>
@@ -2477,10 +2648,10 @@
         <v>4</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="G30" s="2"/>
     </row>
@@ -2491,12 +2662,12 @@
       <c r="E31" s="5"/>
       <c r="F31" s="5"/>
       <c r="G31" s="1" t="s">
-        <v>67</v>
+        <v>76</v>
       </c>
     </row>
     <row r="33" spans="2:8">
       <c r="B33" s="1" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>1</v>
@@ -2505,13 +2676,13 @@
         <v>2</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>58</v>
+        <v>39</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="H33" s="2"/>
     </row>
@@ -2524,13 +2695,13 @@
         <v>4</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="G34" s="6" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="H34" s="2"/>
     </row>
@@ -2542,19 +2713,19 @@
       <c r="F35" s="5"/>
       <c r="G35" s="5"/>
       <c r="H35" s="1" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G34" r:id="rId1" display="test031@demo.cloudnowtech.com " tooltip="mailto:test031@demo.cloudnowtech.com "/>
-    <hyperlink ref="C34" r:id="rId2" display="qa@demo.cloudnowtech.com"/>
-    <hyperlink ref="C20" r:id="rId2" display="qa@demo.cloudnowtech.com"/>
-    <hyperlink ref="C16" r:id="rId2" display="qa@demo.cloudnowtech.com"/>
-    <hyperlink ref="C30" r:id="rId2" display="qa@demo.cloudnowtech.com"/>
-    <hyperlink ref="C12" r:id="rId2" display="qa@demo.cloudnowtech.com"/>
-    <hyperlink ref="C26" r:id="rId2" display="qa@demo.cloudnowtech.com"/>
-    <hyperlink ref="C8" r:id="rId2" display="qa@demo.cloudnowtech.com"/>
+    <hyperlink ref="C8" r:id="rId1" display="qa@demo.cloudnowtech.com"/>
+    <hyperlink ref="C26" r:id="rId1" display="qa@demo.cloudnowtech.com"/>
+    <hyperlink ref="C12" r:id="rId1" display="qa@demo.cloudnowtech.com"/>
+    <hyperlink ref="C30" r:id="rId1" display="qa@demo.cloudnowtech.com"/>
+    <hyperlink ref="C16" r:id="rId1" display="qa@demo.cloudnowtech.com"/>
+    <hyperlink ref="C20" r:id="rId1" display="qa@demo.cloudnowtech.com"/>
+    <hyperlink ref="C34" r:id="rId1" display="qa@demo.cloudnowtech.com"/>
+    <hyperlink ref="G34" r:id="rId2" display="test031@demo.cloudnowtech.com " tooltip="mailto:test031@demo.cloudnowtech.com "/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>